<commit_message>
Remove last line from excel, update wording on get_data
</commit_message>
<xml_diff>
--- a/Parametros.xlsx
+++ b/Parametros.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WampServer\www\TJ-Water\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\TJ-Water\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>Fecha</t>
   </si>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
@@ -507,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L977"/>
+  <dimension ref="A1:L976"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -710,18 +710,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>42993</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13">
-        <v>-7</v>
-      </c>
+      <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F14" s="1"/>
@@ -779,7 +769,7 @@
       <c r="F27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F28" s="1"/>
       <c r="H28" s="1"/>
     </row>
@@ -4574,10 +4564,6 @@
     <row r="976" spans="6:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F976" s="1"/>
       <c r="H976" s="1"/>
-    </row>
-    <row r="977" spans="6:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F977" s="1"/>
-      <c r="H977" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated script once again
The database format has changed (again). The tables created by the
script are:
- history: the full excel sheet
- data: only the latest updated locations
- structure: the structure of the excel file; contains the following
columns:
- id: refers back to the history and data columns
- name: the name of the measure as seen in the excel file
- ind: the index of the measure
- tab: the tab in which the measure is contained
- units: the unit of the measure
</commit_message>
<xml_diff>
--- a/Parametros.xlsx
+++ b/Parametros.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>32°32'01.7"N 117°07'28.6"W</t>
+  </si>
+  <si>
+    <t>Enterococos (kg)</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
   <dimension ref="A1:L977"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -542,7 +545,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
add data in excel
</commit_message>
<xml_diff>
--- a/Parametros.xlsx
+++ b/Parametros.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\TJ-Water\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SteveWang\Desktop\TJ Water\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="A1:L977"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -585,6 +585,30 @@
       <c r="D3">
         <v>8</v>
       </c>
+      <c r="E3">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>33</v>
+      </c>
+      <c r="H3">
+        <v>44</v>
+      </c>
+      <c r="I3">
+        <v>53</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -599,6 +623,30 @@
       <c r="D4">
         <v>9</v>
       </c>
+      <c r="E4">
+        <v>53</v>
+      </c>
+      <c r="F4">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>55</v>
+      </c>
+      <c r="I4">
+        <v>43</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -613,6 +661,30 @@
       <c r="D5">
         <v>5</v>
       </c>
+      <c r="E5">
+        <v>34</v>
+      </c>
+      <c r="F5">
+        <v>44</v>
+      </c>
+      <c r="G5">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>33</v>
+      </c>
+      <c r="I5">
+        <v>33</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -627,6 +699,30 @@
       <c r="D6">
         <v>4</v>
       </c>
+      <c r="E6">
+        <v>55</v>
+      </c>
+      <c r="F6">
+        <v>55</v>
+      </c>
+      <c r="G6">
+        <v>43</v>
+      </c>
+      <c r="H6">
+        <v>44</v>
+      </c>
+      <c r="I6">
+        <v>45</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -641,6 +737,30 @@
       <c r="D7">
         <v>6</v>
       </c>
+      <c r="E7">
+        <v>44</v>
+      </c>
+      <c r="F7">
+        <v>66</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>44</v>
+      </c>
+      <c r="I7">
+        <v>66</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -655,6 +775,30 @@
       <c r="D8">
         <v>7</v>
       </c>
+      <c r="E8">
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <v>77</v>
+      </c>
+      <c r="G8">
+        <v>43</v>
+      </c>
+      <c r="H8">
+        <v>34</v>
+      </c>
+      <c r="I8">
+        <v>43</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -669,6 +813,30 @@
       <c r="D9">
         <v>6</v>
       </c>
+      <c r="E9">
+        <v>55</v>
+      </c>
+      <c r="F9">
+        <v>55</v>
+      </c>
+      <c r="G9">
+        <v>54</v>
+      </c>
+      <c r="H9">
+        <v>54</v>
+      </c>
+      <c r="I9">
+        <v>53</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -683,6 +851,30 @@
       <c r="D10">
         <v>5</v>
       </c>
+      <c r="E10">
+        <v>66</v>
+      </c>
+      <c r="F10">
+        <v>33</v>
+      </c>
+      <c r="G10">
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <v>43</v>
+      </c>
+      <c r="I10">
+        <v>53</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -697,6 +889,30 @@
       <c r="D11">
         <v>6</v>
       </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>44</v>
+      </c>
+      <c r="H11">
+        <v>32</v>
+      </c>
+      <c r="I11">
+        <v>55</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -710,6 +926,30 @@
       </c>
       <c r="D12">
         <v>8</v>
+      </c>
+      <c r="E12">
+        <v>33</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>33</v>
+      </c>
+      <c r="H12">
+        <v>43</v>
+      </c>
+      <c r="I12">
+        <v>22</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>